<commit_message>
Save co2-temp plot work
</commit_message>
<xml_diff>
--- a/GW_Project_Planning.xlsx
+++ b/GW_Project_Planning.xlsx
@@ -24,29 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Tasks</t>
   </si>
   <si>
-    <t>Estimate</t>
-  </si>
-  <si>
-    <t>co2 - temperature comparison chart: most likely a line chart.  Matplotlib or D3?</t>
-  </si>
-  <si>
-    <t>Two pages of comparison charts similar to the comparison page for weather visualization.  This could include some lag, histo, box, temperature, co2, or other charts.</t>
-  </si>
-  <si>
-    <t>Create a few postgres tables for data analysis.  Push these up to Heroku with limited data.</t>
-  </si>
-  <si>
-    <t>Home page: Populate with GW related information.  D3 chart or with GW questions and answers: https://www.nytimes.com/interactive/2017/climate/what-is-climate-change.html</t>
-  </si>
-  <si>
-    <t>Add d3 chart with an array of statements, fact, lies, tweets, or questions that will appear on the screen and then disappear.  This array should cycle continuously.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Updates to the README_Project-GW.md.  </t>
   </si>
   <si>
@@ -54,6 +36,49 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>One chart to tell the story with analysis and linkage to the preparation chart pages.</t>
+  </si>
+  <si>
+    <t>Update to the GitHub README.md</t>
+  </si>
+  <si>
+    <t>This is the README_Project-GW.md file that is displayed on a page then the About link on the home page is clicked.</t>
+  </si>
+  <si>
+    <t>This is the file that sits in the root directory of Project-GW and it will be displayed to anyone visiting the site.  This could have the same information as the "About" readme file or could contain more information.</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>We have the framework for each type of chart, so with the png files it will take 2-3 hours per page.  With a 1-2 more hours pre page for documentation and integration.</t>
+  </si>
+  <si>
+    <t>No idea what this chart will be so no estimate.</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Need update from Aurora and probably meeting with Peleke on 11/27.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make changes to home page.  </t>
+  </si>
+  <si>
+    <t>Create a page or two of preparation charts such as lag plots, temperature, co2,or others.  Make them like the Weather Comparison page which has 4 charts on a page or a series of pages like the 4 weather charts which have one large chart and 4 mini-charts per page.</t>
+  </si>
+  <si>
+    <t>* Add a d3 chart object that only displays an array of comments, questions, or tweets related to global warming.  This may continuously cycle.
+* Add some project explanation to the bottom of the page.</t>
+  </si>
+  <si>
+    <t>Create some PostgreSQL tables for further analysis of the data we have.</t>
+  </si>
+  <si>
+    <t>Depends if we need further analysis and if we have time to do the work for practice and project content.</t>
   </si>
 </sst>
 </file>
@@ -104,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -113,12 +138,45 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -396,14 +454,14 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C11" sqref="C10:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -411,45 +469,84 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorg files and folders
</commit_message>
<xml_diff>
--- a/GW_Project_Planning.xlsx
+++ b/GW_Project_Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Tasks</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Update to the GitHub README.md</t>
   </si>
   <si>
-    <t>This is the README_Project-GW.md file that is displayed on a page then the About link on the home page is clicked.</t>
-  </si>
-  <si>
-    <t>This is the file that sits in the root directory of Project-GW and it will be displayed to anyone visiting the site.  This could have the same information as the "About" readme file or could contain more information.</t>
-  </si>
-  <si>
     <t>Hours</t>
   </si>
   <si>
@@ -60,9 +54,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>Need update from Aurora and probably meeting with Peleke on 11/27.</t>
   </si>
   <si>
     <t xml:space="preserve">Make changes to home page.  </t>
@@ -79,14 +70,77 @@
   </si>
   <si>
     <t>Depends if we need further analysis and if we have time to do the work for practice and project content.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need update from Aurora and probably meeting with Peleke on 11/27.
+Look at making a co2 chart similar to  </t>
+  </si>
+  <si>
+    <t>Clean up folders</t>
+  </si>
+  <si>
+    <t>Aurora to choose countries for co2 and temperature and send to chris.</t>
+  </si>
+  <si>
+    <t>Look for an example chart for temperature.</t>
+  </si>
+  <si>
+    <t>Temperature chart example similar to co2 example?</t>
+  </si>
+  <si>
+    <t>Possible world map with pop-up data like level1 d3 homework.</t>
+  </si>
+  <si>
+    <t>Histograms - what are they supposed to show us?  What parameters to use in creating them?</t>
+  </si>
+  <si>
+    <t>Box plots - what are they supposed to show us?  What parameters to use in creating them?</t>
+  </si>
+  <si>
+    <t>For future learning and possible inclusion in a page of how we got there.</t>
+  </si>
+  <si>
+    <t>Questions for Peleke on 11/30:</t>
+  </si>
+  <si>
+    <t>co2 chart siimilar to area plot for final presentation.</t>
+  </si>
+  <si>
+    <t>temperature chart to show multiple temperature by country as a final chart.</t>
+  </si>
+  <si>
+    <t>Chris and Aurora need to organize and clean up folders and files.</t>
+  </si>
+  <si>
+    <t>This is the README_Project-GW.md file that is displayed on a page when the "About" link on the home page is clicked.</t>
+  </si>
+  <si>
+    <t>This is the file that sits in the root directory of Project-GW GitHub repo, and it will be displayed to anyone visiting the repository.  This could have the same information as the "About" readme file or could contain additional details.</t>
+  </si>
+  <si>
+    <t>Use Matplotlib widgets, D3+, or D3 to create an animated chart.</t>
+  </si>
+  <si>
+    <t>This is a nice to have.</t>
+  </si>
+  <si>
+    <t>Choropleth world and USA maps files availability?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -129,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -143,6 +197,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,16 +509,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C10:C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="47.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="36.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -469,84 +527,165 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B9">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>17</v>
+      <c r="C12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>